<commit_message>
Update to tests and class attributes
</commit_message>
<xml_diff>
--- a/uml_diagram.xlsx
+++ b/uml_diagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevemaddison/Homework/week_02/day_5/codeclan_caraoke/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F0AE836-63F8-274F-8F74-8BF74D6C914F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74274F5B-5B22-924B-A05E-E700E0C63C79}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14500" xr2:uid="{6970BD5C-6A99-F64D-AD5E-C1CEFADD28DC}"/>
   </bookViews>
@@ -25,20 +25,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
-  <si>
-    <t>Room</t>
-  </si>
-  <si>
-    <t>Songs</t>
-  </si>
-  <si>
-    <t>Guests</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>name</t>
   </si>
   <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>capacity</t>
+  </si>
+  <si>
+    <t>artist</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>genre</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>money</t>
+  </si>
+  <si>
     <t>add_songs</t>
   </si>
   <si>
@@ -46,6 +58,48 @@
   </si>
   <si>
     <t>check_out_guests</t>
+  </si>
+  <si>
+    <t>room</t>
+  </si>
+  <si>
+    <t>songs</t>
+  </si>
+  <si>
+    <t>guests</t>
+  </si>
+  <si>
+    <t>Class:</t>
+  </si>
+  <si>
+    <t>Method:</t>
+  </si>
+  <si>
+    <t>Attribute:</t>
+  </si>
+  <si>
+    <t>test name</t>
+  </si>
+  <si>
+    <t>test artist</t>
+  </si>
+  <si>
+    <t>test length</t>
+  </si>
+  <si>
+    <t>test genre</t>
+  </si>
+  <si>
+    <t>test age</t>
+  </si>
+  <si>
+    <t>test money</t>
+  </si>
+  <si>
+    <t>test type</t>
+  </si>
+  <si>
+    <t>test capacity</t>
   </si>
 </sst>
 </file>
@@ -61,15 +115,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -77,12 +137,70 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,52 +515,154 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D5E8DB-E919-C74E-A0FF-662B28BAFFF3}">
-  <dimension ref="B2:F11"/>
+  <dimension ref="A2:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C4" s="6"/>
+      <c r="D4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
+      <c r="C5" s="6"/>
+      <c r="D5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
+      <c r="C6" s="6"/>
+      <c r="D6" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+      <c r="E6" s="6"/>
+      <c r="F6" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>6</v>
+      <c r="E7" s="6"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>